<commit_message>
se finaliza de crear una exposición manual con n registros
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anammoar\Documents\BDDCoreSuraReclamaciones\src\test\resources\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anammoar\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A65480-7855-466C-B1E9-118A986D78EA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9BDDC3-9A05-46FC-A9DE-1883F23197BC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="267" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="750">
   <si>
     <t>VehicleDamage</t>
   </si>
@@ -2245,13 +2245,16 @@
     <t>Pago parcial</t>
   </si>
   <si>
+    <t>9190000041900</t>
+  </si>
+  <si>
     <t>ANA102</t>
   </si>
   <si>
-    <t>9190000042726</t>
-  </si>
-  <si>
-    <t>476097</t>
+    <t>9190000043941</t>
+  </si>
+  <si>
+    <t>1009022</t>
   </si>
   <si>
     <t>0%</t>
@@ -2260,22 +2263,43 @@
     <t>47</t>
   </si>
   <si>
-    <t>09092019152656784</t>
-  </si>
-  <si>
-    <t>CUS165</t>
-  </si>
-  <si>
-    <t>7784010</t>
-  </si>
-  <si>
-    <t>09092019153030740</t>
-  </si>
-  <si>
-    <t>5466359</t>
-  </si>
-  <si>
-    <t>09092019153313187</t>
+    <t>19092019151614856</t>
+  </si>
+  <si>
+    <t>000</t>
+  </si>
+  <si>
+    <t>6182888</t>
+  </si>
+  <si>
+    <t>19092019151743386</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>6305023</t>
+  </si>
+  <si>
+    <t>19092019151910884</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>7771985</t>
+  </si>
+  <si>
+    <t>19092019152039526</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>766016</t>
+  </si>
+  <si>
+    <t>19092019152207527</t>
   </si>
 </sst>
 </file>
@@ -2488,7 +2512,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -2551,6 +2575,13 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2560,6 +2591,8 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -2567,6 +2600,9 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
@@ -3617,46 +3653,46 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:AC2001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" style="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" style="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.85546875" style="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" style="35" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.140625" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.28515625" style="20" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.140625" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="31.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15.7109375" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.7109375" style="4" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="41.140625" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="29.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.28515625" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.85546875" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.42578125" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="52.140625" style="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.42578125" style="19" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" style="33" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18" style="36" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="9.85546875" style="40" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="7.42578125" style="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19" style="5" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="11.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="16.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="26.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.85546875" style="4" collapsed="1"/>
-    <col min="28" max="28" width="13.85546875" style="4" customWidth="1" collapsed="1"/>
-    <col min="29" max="16384" width="8.85546875" style="4" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="31" width="29.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="32" width="10.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="32" width="30.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="38" width="17.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="19" width="28.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="20" width="20.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="19" width="28.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="31.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="19" width="15.7109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="4" width="12.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="19" width="41.140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="4" width="29.140625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="19" width="15.28515625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="19" width="9.85546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="19" width="13.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="19" width="52.140625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="19" width="13.42578125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="33" width="16.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="39" width="18.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="45" width="9.85546875" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="37" width="7.42578125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="5" width="19.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="11.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="16.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="26.140625" collapsed="true"/>
+    <col min="27" max="27" style="4" width="8.85546875" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="4" width="13.85546875" collapsed="true"/>
+    <col min="29" max="16384" style="4" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>8</v>
       </c>
@@ -3717,253 +3753,407 @@
       <c r="T1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="39" t="s">
+      <c r="U1" s="44" t="s">
         <v>17</v>
       </c>
       <c r="V1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="38" t="s">
+      <c r="W1" s="41" t="s">
         <v>723</v>
       </c>
       <c r="X1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="38" t="s">
+      <c r="Y1" s="41" t="s">
         <v>704</v>
       </c>
       <c r="Z1" s="27" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
-        <v>732</v>
-      </c>
-      <c r="B2" s="32" t="s">
+    <row r="2">
+      <c r="A2" t="s" s="31">
+        <v>733</v>
+      </c>
+      <c r="B2" t="s" s="32">
         <v>729</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" t="s" s="32">
         <v>50</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" t="s" s="38">
         <v>0</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" t="s" s="19">
         <v>164</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" t="s" s="20">
         <v>21</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" t="s" s="19">
         <v>164</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" t="s" s="4">
         <v>21</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" t="s" s="19">
         <v>215</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" t="s" s="4">
         <v>711</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" t="s" s="19">
         <v>370</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" t="s" s="19">
         <v>506</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" t="s" s="4">
         <v>505</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" t="s" s="19">
+        <v>734</v>
+      </c>
+      <c r="P2" t="s" s="19">
+        <v>735</v>
+      </c>
+      <c r="Q2" t="s" s="19">
+        <v>622</v>
+      </c>
+      <c r="R2" t="s" s="19">
+        <v>622</v>
+      </c>
+      <c r="S2" t="s" s="33">
+        <v>681</v>
+      </c>
+      <c r="T2" t="s" s="39">
+        <v>673</v>
+      </c>
+      <c r="U2" t="s" s="45">
+        <v>736</v>
+      </c>
+      <c r="V2" t="s" s="37">
+        <v>737</v>
+      </c>
+      <c r="X2" t="s" s="4">
+        <v>730</v>
+      </c>
+      <c r="Y2" t="s" s="4">
+        <v>706</v>
+      </c>
+      <c r="Z2" t="s" s="4">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="31">
         <v>733</v>
       </c>
-      <c r="P2" s="19" t="s">
-        <v>734</v>
-      </c>
-      <c r="Q2" s="19" t="s">
-        <v>622</v>
-      </c>
-      <c r="R2" s="19" t="s">
-        <v>622</v>
-      </c>
-      <c r="S2" s="33" t="s">
+      <c r="B3" t="s" s="32">
+        <v>738</v>
+      </c>
+      <c r="C3" t="s" s="32">
+        <v>50</v>
+      </c>
+      <c r="D3" t="s" s="38">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s" s="19">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G3" t="s" s="19">
+        <v>207</v>
+      </c>
+      <c r="H3" t="s" s="4">
+        <v>122</v>
+      </c>
+      <c r="I3" t="s" s="19">
+        <v>215</v>
+      </c>
+      <c r="J3" t="s" s="4">
+        <v>711</v>
+      </c>
+      <c r="K3" t="s" s="19">
+        <v>370</v>
+      </c>
+      <c r="L3" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s" s="19">
+        <v>506</v>
+      </c>
+      <c r="N3" t="s" s="4">
+        <v>505</v>
+      </c>
+      <c r="O3" t="s" s="19">
+        <v>739</v>
+      </c>
+      <c r="P3" t="s" s="19">
+        <v>735</v>
+      </c>
+      <c r="Q3" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="R3" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s" s="33">
         <v>681</v>
       </c>
-      <c r="T2" s="36" t="s">
+      <c r="T3" t="s" s="39">
         <v>673</v>
       </c>
-      <c r="U2" s="40" t="s">
+      <c r="U3" t="s" s="45">
+        <v>736</v>
+      </c>
+      <c r="V3" t="s" s="37">
+        <v>740</v>
+      </c>
+      <c r="X3" t="s" s="4">
+        <v>730</v>
+      </c>
+      <c r="Y3" t="s" s="4">
+        <v>706</v>
+      </c>
+      <c r="Z3" t="s" s="4">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="31">
+        <v>733</v>
+      </c>
+      <c r="B4" t="s" s="32">
+        <v>741</v>
+      </c>
+      <c r="C4" t="s" s="32">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s" s="38">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s" s="19">
+        <v>166</v>
+      </c>
+      <c r="F4" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G4" t="s" s="19">
+        <v>207</v>
+      </c>
+      <c r="H4" t="s" s="4">
+        <v>122</v>
+      </c>
+      <c r="I4" t="s" s="19">
+        <v>215</v>
+      </c>
+      <c r="J4" t="s" s="4">
+        <v>711</v>
+      </c>
+      <c r="K4" t="s" s="19">
+        <v>370</v>
+      </c>
+      <c r="L4" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s" s="19">
+        <v>506</v>
+      </c>
+      <c r="N4" t="s" s="4">
+        <v>505</v>
+      </c>
+      <c r="O4" t="s" s="19">
+        <v>742</v>
+      </c>
+      <c r="P4" t="s" s="19">
         <v>735</v>
       </c>
-      <c r="V2" s="34" t="s">
+      <c r="Q4" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="R4" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="S4" t="s" s="33">
+        <v>681</v>
+      </c>
+      <c r="T4" t="s" s="39">
+        <v>673</v>
+      </c>
+      <c r="U4" t="s" s="45">
         <v>736</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="V4" t="s" s="37">
+        <v>743</v>
+      </c>
+      <c r="X4" t="s" s="4">
         <v>730</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y4" t="s" s="4">
         <v>706</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z4" t="s" s="4">
         <v>653</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>732</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>737</v>
-      </c>
-      <c r="C3" s="32" t="s">
+    <row r="5">
+      <c r="A5" t="s" s="31">
+        <v>733</v>
+      </c>
+      <c r="B5" t="s" s="32">
+        <v>744</v>
+      </c>
+      <c r="C5" t="s" s="32">
         <v>50</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D5" t="s" s="38">
         <v>0</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E5" t="s" s="19">
         <v>166</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F5" t="s" s="20">
         <v>76</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G5" t="s" s="19">
         <v>207</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H5" t="s" s="4">
         <v>122</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I5" t="s" s="19">
         <v>215</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J5" t="s" s="4">
         <v>711</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K5" t="s" s="19">
         <v>370</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L5" t="s" s="4">
         <v>22</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="M5" t="s" s="19">
         <v>506</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N5" t="s" s="4">
         <v>505</v>
       </c>
-      <c r="O3" s="19" t="s">
-        <v>738</v>
-      </c>
-      <c r="P3" s="19" t="s">
-        <v>734</v>
-      </c>
-      <c r="Q3" s="19" t="s">
+      <c r="O5" t="s" s="19">
+        <v>745</v>
+      </c>
+      <c r="P5" t="s" s="19">
+        <v>735</v>
+      </c>
+      <c r="Q5" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R5" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="S3" s="33" t="s">
+      <c r="S5" t="s" s="33">
         <v>681</v>
       </c>
-      <c r="T3" s="36" t="s">
+      <c r="T5" t="s" s="39">
         <v>673</v>
       </c>
-      <c r="U3" s="40" t="s">
+      <c r="U5" t="s" s="45">
+        <v>736</v>
+      </c>
+      <c r="V5" t="s" s="37">
+        <v>746</v>
+      </c>
+      <c r="X5" t="s" s="4">
+        <v>730</v>
+      </c>
+      <c r="Y5" t="s" s="4">
+        <v>706</v>
+      </c>
+      <c r="Z5" t="s" s="4">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="31">
+        <v>733</v>
+      </c>
+      <c r="B6" t="s" s="32">
+        <v>747</v>
+      </c>
+      <c r="C6" t="s" s="32">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s" s="38">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s" s="19">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s" s="20">
+        <v>76</v>
+      </c>
+      <c r="G6" t="s" s="19">
+        <v>207</v>
+      </c>
+      <c r="H6" t="s" s="4">
+        <v>122</v>
+      </c>
+      <c r="I6" t="s" s="19">
+        <v>215</v>
+      </c>
+      <c r="J6" t="s" s="4">
+        <v>711</v>
+      </c>
+      <c r="K6" t="s" s="19">
+        <v>370</v>
+      </c>
+      <c r="L6" t="s" s="4">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s" s="19">
+        <v>506</v>
+      </c>
+      <c r="N6" t="s" s="4">
+        <v>505</v>
+      </c>
+      <c r="O6" t="s" s="19">
+        <v>748</v>
+      </c>
+      <c r="P6" t="s" s="19">
         <v>735</v>
       </c>
-      <c r="V3" s="34" t="s">
-        <v>739</v>
-      </c>
-      <c r="X3" s="4" t="s">
+      <c r="Q6" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="R6" t="s" s="19">
+        <v>23</v>
+      </c>
+      <c r="S6" t="s" s="33">
+        <v>681</v>
+      </c>
+      <c r="T6" t="s" s="39">
+        <v>673</v>
+      </c>
+      <c r="U6" t="s" s="45">
+        <v>736</v>
+      </c>
+      <c r="V6" t="s" s="37">
+        <v>749</v>
+      </c>
+      <c r="X6" t="s" s="4">
         <v>730</v>
       </c>
-      <c r="Y3" s="4" t="s">
+      <c r="Y6" t="s" s="4">
         <v>706</v>
       </c>
-      <c r="Z3" s="4" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>732</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>731</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>215</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="K4" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="19" t="s">
-        <v>506</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="O4" s="19" t="s">
-        <v>740</v>
-      </c>
-      <c r="P4" s="19" t="s">
-        <v>734</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="33" t="s">
-        <v>681</v>
-      </c>
-      <c r="T4" s="36" t="s">
-        <v>673</v>
-      </c>
-      <c r="U4" s="40" t="s">
-        <v>735</v>
-      </c>
-      <c r="V4" s="34" t="s">
-        <v>741</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>730</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>706</v>
-      </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Z6" t="s" s="4">
         <v>653</v>
       </c>
     </row>
@@ -4005,7 +4195,7 @@
     <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000009000000}">
           <x14:formula1>
@@ -4030,29 +4220,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="36.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="41.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.85546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="48" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="30.85546875" style="6" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" style="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="40.42578125" style="6" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="37.140625" style="6" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="65.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="12" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="27.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="6" width="36.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="6" width="8.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="48.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="6" width="30.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="6" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" style="6" width="40.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="6" width="37.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="65.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="27.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="9.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="45" x14ac:dyDescent="0.25">
@@ -4128,10 +4318,10 @@
       <c r="AF1" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="37" t="s">
+      <c r="AH1" s="40" t="s">
         <v>214</v>
       </c>
-      <c r="AI1" s="37" t="s">
+      <c r="AI1" s="40" t="s">
         <v>205</v>
       </c>
     </row>
@@ -5250,10 +5440,10 @@
       <c r="J19" t="s">
         <v>728</v>
       </c>
-      <c r="K19" s="41" t="s">
+      <c r="K19" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="L19" s="41">
+      <c r="L19" s="46">
         <v>80</v>
       </c>
       <c r="Q19" s="12" t="s">

</xml_diff>

<commit_message>
Se adiciona generar póliza, se actualiza generar numeros aleatorios, taller de reparación
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5614" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5664" uniqueCount="1187">
   <si>
     <t>VehicleDamage</t>
   </si>
@@ -3590,6 +3590,27 @@
   </si>
   <si>
     <t>02072021160439006</t>
+  </si>
+  <si>
+    <t>9210000058099</t>
+  </si>
+  <si>
+    <t>CUS165</t>
+  </si>
+  <si>
+    <t>15530</t>
+  </si>
+  <si>
+    <t>12072021135139382</t>
+  </si>
+  <si>
+    <t>ACJB038</t>
+  </si>
+  <si>
+    <t>509734</t>
+  </si>
+  <si>
+    <t>12072021135140586</t>
   </si>
 </sst>
 </file>
@@ -5064,10 +5085,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="31">
-        <v>1174</v>
+        <v>1180</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>732</v>
+        <v>1181</v>
       </c>
       <c r="C2" t="s" s="32">
         <v>50</v>
@@ -5106,7 +5127,7 @@
         <v>505</v>
       </c>
       <c r="O2" t="s" s="19">
-        <v>1175</v>
+        <v>1182</v>
       </c>
       <c r="P2" t="s" s="19">
         <v>736</v>
@@ -5127,7 +5148,7 @@
         <v>737</v>
       </c>
       <c r="V2" t="s" s="37">
-        <v>1176</v>
+        <v>1183</v>
       </c>
       <c r="X2" t="s" s="4">
         <v>730</v>
@@ -5141,10 +5162,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="31">
-        <v>1174</v>
+        <v>1180</v>
       </c>
       <c r="B3" t="s" s="32">
-        <v>1177</v>
+        <v>1184</v>
       </c>
       <c r="C3" t="s" s="32">
         <v>50</v>
@@ -5183,7 +5204,7 @@
         <v>505</v>
       </c>
       <c r="O3" t="s" s="19">
-        <v>1178</v>
+        <v>1185</v>
       </c>
       <c r="P3" t="s" s="19">
         <v>736</v>
@@ -5204,7 +5225,7 @@
         <v>737</v>
       </c>
       <c r="V3" t="s" s="37">
-        <v>1179</v>
+        <v>1186</v>
       </c>
       <c r="X3" t="s" s="4">
         <v>730</v>

</xml_diff>

<commit_message>
Solución de deuda tecnica Sonar
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5664" uniqueCount="1187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5714" uniqueCount="1193">
   <si>
     <t>VehicleDamage</t>
   </si>
@@ -3611,6 +3611,24 @@
   </si>
   <si>
     <t>12072021135140586</t>
+  </si>
+  <si>
+    <t>9210000058132</t>
+  </si>
+  <si>
+    <t>346254</t>
+  </si>
+  <si>
+    <t>13072021150826854</t>
+  </si>
+  <si>
+    <t>JXKB804</t>
+  </si>
+  <si>
+    <t>16474</t>
+  </si>
+  <si>
+    <t>13072021150827561</t>
   </si>
 </sst>
 </file>
@@ -5085,7 +5103,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="31">
-        <v>1180</v>
+        <v>1187</v>
       </c>
       <c r="B2" t="s" s="32">
         <v>1181</v>
@@ -5127,7 +5145,7 @@
         <v>505</v>
       </c>
       <c r="O2" t="s" s="19">
-        <v>1182</v>
+        <v>1188</v>
       </c>
       <c r="P2" t="s" s="19">
         <v>736</v>
@@ -5148,7 +5166,7 @@
         <v>737</v>
       </c>
       <c r="V2" t="s" s="37">
-        <v>1183</v>
+        <v>1189</v>
       </c>
       <c r="X2" t="s" s="4">
         <v>730</v>
@@ -5162,10 +5180,10 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="31">
-        <v>1180</v>
+        <v>1187</v>
       </c>
       <c r="B3" t="s" s="32">
-        <v>1184</v>
+        <v>1190</v>
       </c>
       <c r="C3" t="s" s="32">
         <v>50</v>
@@ -5204,7 +5222,7 @@
         <v>505</v>
       </c>
       <c r="O3" t="s" s="19">
-        <v>1185</v>
+        <v>1191</v>
       </c>
       <c r="P3" t="s" s="19">
         <v>736</v>
@@ -5225,7 +5243,7 @@
         <v>737</v>
       </c>
       <c r="V3" t="s" s="37">
-        <v>1186</v>
+        <v>1192</v>
       </c>
       <c r="X3" t="s" s="4">
         <v>730</v>

</xml_diff>

<commit_message>
se ajusta time out en automatización
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="486">
   <si>
     <t>Siniestro</t>
   </si>
@@ -1488,6 +1488,18 @@
   </si>
   <si>
     <t>28102021142455875</t>
+  </si>
+  <si>
+    <t>9210000060434</t>
+  </si>
+  <si>
+    <t>20122021092316714</t>
+  </si>
+  <si>
+    <t>NDEJ119</t>
+  </si>
+  <si>
+    <t>20122021092317214</t>
   </si>
 </sst>
 </file>
@@ -3153,7 +3165,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>474</v>
@@ -3224,7 +3236,7 @@
         <v>468</v>
       </c>
       <c r="V2" s="49" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="W2" s="18">
         <v>44491</v>
@@ -3242,10 +3254,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>86</v>
@@ -3313,7 +3325,7 @@
         <v>469</v>
       </c>
       <c r="V3" s="26" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="W3" s="27">
         <v>44491</v>

</xml_diff>

<commit_message>
se ajustan tags de ejecución
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="490">
   <si>
     <t>Siniestro</t>
   </si>
@@ -1500,6 +1500,18 @@
   </si>
   <si>
     <t>20122021092317214</t>
+  </si>
+  <si>
+    <t>9220000060631</t>
+  </si>
+  <si>
+    <t>11012022145403149</t>
+  </si>
+  <si>
+    <t>QMZX401</t>
+  </si>
+  <si>
+    <t>11012022145403674</t>
   </si>
 </sst>
 </file>
@@ -3165,7 +3177,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>474</v>
@@ -3236,7 +3248,7 @@
         <v>468</v>
       </c>
       <c r="V2" s="49" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="W2" s="18">
         <v>44491</v>
@@ -3254,10 +3266,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>86</v>
@@ -3325,7 +3337,7 @@
         <v>469</v>
       </c>
       <c r="V3" s="26" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="W3" s="27">
         <v>44491</v>

</xml_diff>

<commit_message>
se ajusta excel en caso de prueba pago masivo
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="477">
   <si>
     <t>Siniestro</t>
   </si>
@@ -1454,54 +1454,12 @@
     <t>ATT</t>
   </si>
   <si>
-    <t>FACT202</t>
-  </si>
-  <si>
     <t>parcial</t>
   </si>
   <si>
-    <t>FACT203</t>
-  </si>
-  <si>
-    <t>9210000059917</t>
-  </si>
-  <si>
     <t>CUS165</t>
   </si>
   <si>
-    <t>JIOK954</t>
-  </si>
-  <si>
-    <t>9210000059921</t>
-  </si>
-  <si>
-    <t>BWEW701</t>
-  </si>
-  <si>
-    <t>9210000059922</t>
-  </si>
-  <si>
-    <t>28102021142401665</t>
-  </si>
-  <si>
-    <t>CMNY902</t>
-  </si>
-  <si>
-    <t>28102021142455875</t>
-  </si>
-  <si>
-    <t>9210000060434</t>
-  </si>
-  <si>
-    <t>20122021092316714</t>
-  </si>
-  <si>
-    <t>NDEJ119</t>
-  </si>
-  <si>
-    <t>20122021092317214</t>
-  </si>
-  <si>
     <t>9220000060631</t>
   </si>
   <si>
@@ -1512,6 +1470,9 @@
   </si>
   <si>
     <t>11012022145403674</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1483,7 @@
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1581,6 +1542,24 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1755,7 +1734,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1818,6 +1797,12 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2063,13 +2048,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A21:A1000"/>
+  <dimension ref="A21:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" customWidth="true" width="7.75" collapsed="true"/>
+    <col min="1" max="26" width="7.75" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3062,37 +3047,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z834"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="31.75" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="21.625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="43.5" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="25.5" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="13.375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="14.625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="14.25" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="11.75" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="15.25" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="11.75" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="14.625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="15.75" collapsed="true"/>
-    <col min="21" max="22" customWidth="true" width="8.625" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="16.625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="14.625" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="22.875" collapsed="true"/>
+    <col min="1" max="1" width="19.875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="36.25" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="43.5" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="25.5" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="14.25" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="11.75" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15.25" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.75" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="14.625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="15.75" customWidth="1" collapsed="1"/>
+    <col min="21" max="22" width="8.625" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.625" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="22.875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -3177,10 +3162,10 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>86</v>
@@ -3190,18 +3175,18 @@
         <v>VehicleDamage</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>115</v>
+        <v>214</v>
       </c>
       <c r="F2" s="13" t="str">
         <f>IF(ISBLANK(E2)," ",INDEX(CoberturaCode,MATCH(E2,Cobertura,0)))</f>
-        <v>PADanosCov</v>
+        <v>PARCCov</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>115</v>
+        <v>226</v>
       </c>
       <c r="H2" s="13" t="str">
         <f t="array" ref="H2">IF(ISBLANK(G2)," ",INDEX(SubcoberturaCode,MATCH(G2,Subcobertura,0)))</f>
-        <v>PADanosCov</v>
+        <v>PARCCov-veh</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>45</v>
@@ -3210,19 +3195,19 @@
         <f t="array" ref="J2">IF(ISBLANK(I2)," ",INDEX(CostTypeCode,MATCH(I2,CostType,0)))</f>
         <v>claimcost</v>
       </c>
-      <c r="K2" s="12" t="s">
-        <v>244</v>
+      <c r="K2" s="53" t="s">
+        <v>260</v>
       </c>
       <c r="L2" s="13" t="str">
         <f t="array" ref="L2">IF(ISBLANK(K2)," ",INDEX(CostCategoryCode,MATCH(K2,CostCategory,0)))</f>
-        <v>PAPerParcDanAutoTaller_Ext</v>
+        <v>PAPerdTotDanPagEfec_Ext</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="N2" s="13" t="str">
-        <f t="array" ref="N2">IF(ISBLANK(M2)," ",INDEX(TipoPagoCode,MATCH(M2,TipoPago,0)))</f>
-        <v>Partial</v>
+        <f>IF(ISBLANK(M2)," ",INDEX(TipoPagoCode,MATCH(M2,TipoPago,0)))</f>
+        <v>Final</v>
       </c>
       <c r="O2" s="14">
         <v>100000</v>
@@ -3248,13 +3233,13 @@
         <v>468</v>
       </c>
       <c r="V2" s="49" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="W2" s="18">
         <v>44491</v>
       </c>
       <c r="X2" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="Y2" s="12" t="s">
         <v>57</v>
@@ -3266,10 +3251,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>86</v>
@@ -3279,18 +3264,18 @@
         <v>VehicleDamage</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>214</v>
+        <v>115</v>
       </c>
       <c r="F3" s="13" t="str">
         <f t="array" ref="F3">IF(ISBLANK(E3)," ",INDEX(CoberturaCode,MATCH(E3,Cobertura,0)))</f>
-        <v>PARCCov</v>
+        <v>PADanosCov</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>226</v>
+        <v>115</v>
       </c>
       <c r="H3" s="13" t="str">
         <f t="array" ref="H3">IF(ISBLANK(G3)," ",INDEX(SubcoberturaCode,MATCH(G3,Subcobertura,0)))</f>
-        <v>PARCCov-veh</v>
+        <v>PADanosCov</v>
       </c>
       <c r="I3" s="13" t="s">
         <v>45</v>
@@ -3299,19 +3284,19 @@
         <f t="array" ref="J3">IF(ISBLANK(I3)," ",INDEX(CostTypeCode,MATCH(I3,CostType,0)))</f>
         <v>claimcost</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>244</v>
+      <c r="K3" s="52" t="s">
+        <v>64</v>
       </c>
       <c r="L3" s="13" t="str">
         <f t="array" ref="L3">IF(ISBLANK(K3)," ",INDEX(CostCategoryCode,MATCH(K3,CostCategory,0)))</f>
-        <v>PAPerParcDanAutoTaller_Ext</v>
+        <v>GENDanosVehiculosClaimcost_Ext</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="N3" s="13" t="str">
         <f t="array" ref="N3">IF(ISBLANK(M3)," ",INDEX(TipoPagoCode,MATCH(M3,TipoPago,0)))</f>
-        <v>Partial</v>
+        <v>Final</v>
       </c>
       <c r="O3" s="24">
         <v>100000</v>
@@ -3337,13 +3322,13 @@
         <v>469</v>
       </c>
       <c r="V3" s="26" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="W3" s="27">
         <v>44491</v>
       </c>
       <c r="X3" s="28" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="Y3" s="12" t="s">
         <v>57</v>
@@ -3402,70 +3387,74 @@
       <c r="Q15" s="30"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="50"/>
       <c r="O16" s="29"/>
       <c r="Q16" s="30"/>
     </row>
-    <row r="17" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="51" t="s">
+        <v>476</v>
+      </c>
       <c r="O17" s="29"/>
       <c r="Q17" s="30"/>
     </row>
-    <row r="18" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O18" s="29"/>
       <c r="Q18" s="30"/>
     </row>
-    <row r="19" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O19" s="29"/>
       <c r="Q19" s="30"/>
     </row>
-    <row r="20" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O20" s="29"/>
       <c r="Q20" s="30"/>
     </row>
-    <row r="21" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O21" s="29"/>
       <c r="Q21" s="30"/>
     </row>
-    <row r="22" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O22" s="29"/>
       <c r="Q22" s="30"/>
     </row>
-    <row r="23" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O23" s="29"/>
       <c r="Q23" s="30"/>
     </row>
-    <row r="24" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O24" s="29"/>
       <c r="Q24" s="30"/>
     </row>
-    <row r="25" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O25" s="29"/>
       <c r="Q25" s="30"/>
     </row>
-    <row r="26" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O26" s="29"/>
       <c r="Q26" s="30"/>
     </row>
-    <row r="27" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O27" s="29"/>
       <c r="Q27" s="30"/>
     </row>
-    <row r="28" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O28" s="29"/>
       <c r="Q28" s="30"/>
     </row>
-    <row r="29" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O29" s="29"/>
       <c r="Q29" s="30"/>
     </row>
-    <row r="30" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O30" s="29"/>
       <c r="Q30" s="30"/>
     </row>
-    <row r="31" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O31" s="29"/>
       <c r="Q31" s="30"/>
     </row>
-    <row r="32" spans="15:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="O32" s="29"/>
       <c r="Q32" s="30"/>
     </row>
@@ -6728,7 +6717,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -6754,34 +6743,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.5" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="9.125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="31.875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="36.625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="7.75" collapsed="true"/>
-    <col min="8" max="9" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="9.75" collapsed="true"/>
-    <col min="13" max="14" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="10.625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="35.375" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="32.5" collapsed="true"/>
-    <col min="19" max="22" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="6.5" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="7.125" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="57.5" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="9.75" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="28" max="28" customWidth="true" width="10.5" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="24.375" collapsed="true"/>
-    <col min="30" max="31" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="15.625" collapsed="true"/>
-    <col min="33" max="33" customWidth="true" width="8.0" collapsed="true"/>
-    <col min="34" max="34" customWidth="true" width="16.25" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="8.125" collapsed="true"/>
+    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="36.625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.75" customWidth="1" collapsed="1"/>
+    <col min="8" max="9" width="8" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="42" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.75" customWidth="1" collapsed="1"/>
+    <col min="13" max="14" width="8" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="10.625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="35.375" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="32.5" customWidth="1" collapsed="1"/>
+    <col min="19" max="22" width="8" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="6.5" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="7.125" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="57.5" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.75" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="10" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="10.5" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="24.375" customWidth="1" collapsed="1"/>
+    <col min="30" max="31" width="8" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="15.625" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="8" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="16.25" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="8.125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se ajustan tangs de ejecución y tiempo de espera
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="480">
   <si>
     <t>Siniestro</t>
   </si>
@@ -1470,6 +1470,18 @@
   </si>
   <si>
     <t>12012022124510939</t>
+  </si>
+  <si>
+    <t>9220000060656</t>
+  </si>
+  <si>
+    <t>12012022135937421</t>
+  </si>
+  <si>
+    <t>MYZB664</t>
+  </si>
+  <si>
+    <t>12012022135938026</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2047,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="26" width="7.75" customWidth="1" collapsed="1"/>
+    <col min="1" max="26" customWidth="true" width="7.75" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3034,32 +3046,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="21.625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="43.5" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="25.5" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="14.25" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="11.75" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15.25" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="11.75" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="14.625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="15.75" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24.125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="14.625" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="22.875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.75" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="21.625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="43.5" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="25.5" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="13.375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="14.625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.25" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="11.75" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="15.25" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="11.75" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="14.625" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="15.75" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="8.625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="24.125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="16.625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="14.625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="22.875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -3144,7 +3156,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>471</v>
@@ -3215,7 +3227,7 @@
         <v>468</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="W2" s="18">
         <v>44562</v>
@@ -3233,10 +3245,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>86</v>
@@ -3304,7 +3316,7 @@
         <v>469</v>
       </c>
       <c r="V3" s="25" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="W3" s="26">
         <v>44562</v>
@@ -6721,34 +6733,34 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="36.625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="7.75" customWidth="1" collapsed="1"/>
-    <col min="8" max="9" width="8" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="42" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.75" customWidth="1" collapsed="1"/>
-    <col min="13" max="14" width="8" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="10.625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="35.375" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="32.5" customWidth="1" collapsed="1"/>
-    <col min="19" max="22" width="8" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="6.5" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="7.125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="57.5" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.75" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="10" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="10.5" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="24.375" customWidth="1" collapsed="1"/>
-    <col min="30" max="31" width="8" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="15.625" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="8" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="16.25" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="8.125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="36.625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="7.75" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="9.75" collapsed="true"/>
+    <col min="13" max="14" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" width="10.625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="35.375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="32.5" collapsed="true"/>
+    <col min="19" max="22" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="6.5" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="7.125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="57.5" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="9.75" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="24.375" collapsed="true"/>
+    <col min="30" max="31" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="15.625" collapsed="true"/>
+    <col min="33" max="33" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="34" max="34" customWidth="true" width="16.25" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="8.125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:35" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se ajustan tags de pruebas
</commit_message>
<xml_diff>
--- a/src/test/resources/files/PlantillaPagosMasivos.xlsx
+++ b/src/test/resources/files/PlantillaPagosMasivos.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="484">
   <si>
     <t>Siniestro</t>
   </si>
@@ -1482,6 +1482,18 @@
   </si>
   <si>
     <t>12012022135938026</t>
+  </si>
+  <si>
+    <t>9220000061149</t>
+  </si>
+  <si>
+    <t>22022022142714783</t>
+  </si>
+  <si>
+    <t>DNOR633</t>
+  </si>
+  <si>
+    <t>22022022142715814</t>
   </si>
 </sst>
 </file>
@@ -3156,7 +3168,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>471</v>
@@ -3227,7 +3239,7 @@
         <v>468</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="W2" s="18">
         <v>44562</v>
@@ -3245,10 +3257,10 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>86</v>
@@ -3316,7 +3328,7 @@
         <v>469</v>
       </c>
       <c r="V3" s="25" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="W3" s="26">
         <v>44562</v>

</xml_diff>